<commit_message>
using migrate to import marathons
</commit_message>
<xml_diff>
--- a/data/marathons.xlsx
+++ b/data/marathons.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="462">
   <si>
     <t>Datum</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Cairns</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
     <t>http://www.crocodile-trophy.com/</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>Willingen</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>http://www.bike-festival-willingen.de/</t>
   </si>
   <si>
@@ -745,9 +739,6 @@
     <t>Balatonfured</t>
   </si>
   <si>
-    <t>Hun</t>
-  </si>
-  <si>
     <t>Duna Marathon</t>
   </si>
   <si>
@@ -760,9 +751,6 @@
     <t>Niederdorf-Villabassa</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>Bike Marathon Garda Trentino</t>
   </si>
   <si>
@@ -823,9 +811,6 @@
     <t>Luxemburg-Amsterdam</t>
   </si>
   <si>
-    <t>Lux-Ned</t>
-  </si>
-  <si>
     <t>Transmarocaine</t>
   </si>
   <si>
@@ -892,9 +877,6 @@
     <t>Assen</t>
   </si>
   <si>
-    <t>23-24/3/13</t>
-  </si>
-  <si>
     <t>Gert Jan Theunisse Classic</t>
   </si>
   <si>
@@ -976,9 +958,6 @@
     <t>Bucklige Welt/Krumbach</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>Alpentour Trophy</t>
   </si>
   <si>
@@ -1129,9 +1108,6 @@
     <t>Archensee</t>
   </si>
   <si>
-    <t>O / IT</t>
-  </si>
-  <si>
     <t>La Lozerienne</t>
   </si>
   <si>
@@ -1201,9 +1177,6 @@
     <t>Cordoba</t>
   </si>
   <si>
-    <t>Spa</t>
-  </si>
-  <si>
     <t>http://www.andaluciabikerace.com/</t>
   </si>
   <si>
@@ -1240,18 +1213,12 @@
     <t>Llanwrtyd Wells</t>
   </si>
   <si>
-    <t>Wales</t>
-  </si>
-  <si>
     <t>Iron Bike Race</t>
   </si>
   <si>
     <t>Einsiedeln</t>
   </si>
   <si>
-    <t>Zwi</t>
-  </si>
-  <si>
     <t>O Tour Bike Challenge  UCI series</t>
   </si>
   <si>
@@ -1264,9 +1231,6 @@
     <t>Capetown</t>
   </si>
   <si>
-    <t>Z Afr</t>
-  </si>
-  <si>
     <t>Aletisch Bike Marathon </t>
   </si>
   <si>
@@ -1315,9 +1279,6 @@
     <t>Rorschach</t>
   </si>
   <si>
-    <t>Zwi-Oost-Ita</t>
-  </si>
-  <si>
     <t>Grand Raid Cristalp</t>
   </si>
   <si>
@@ -1408,13 +1369,37 @@
     <t>Sudety Bike Challenge</t>
   </si>
   <si>
-    <t>http://www.o2bikers.com/pg.asp?pageID=272&amp;lgid=nl</t>
-  </si>
-  <si>
     <t>http://www.zillertal-bikechallenge.com/</t>
   </si>
   <si>
     <t>LCMT</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>AUS</t>
   </si>
 </sst>
 </file>
@@ -2250,10 +2235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H193"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A192" sqref="A192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2300,13 +2285,13 @@
         <v>866</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>461</v>
       </c>
       <c r="G2">
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2314,10 +2299,10 @@
         <v>41404</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3">
         <v>250</v>
@@ -2326,7 +2311,7 @@
         <v>7500</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -2337,25 +2322,25 @@
         <v>41383</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
       </c>
       <c r="E4">
         <v>4032</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2363,10 +2348,10 @@
         <v>41403</v>
       </c>
       <c r="B5" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>413</v>
@@ -2375,7 +2360,7 @@
         <v>6388</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2383,16 +2368,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
       </c>
       <c r="D6">
         <v>333</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -2400,10 +2385,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
       </c>
       <c r="D7">
         <v>565</v>
@@ -2412,7 +2397,7 @@
         <v>10000</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -2423,10 +2408,10 @@
         <v>41454</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
       </c>
       <c r="D8">
         <v>335</v>
@@ -2435,7 +2420,7 @@
         <v>9370</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -2446,10 +2431,10 @@
         <v>41482</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
       </c>
       <c r="D9">
         <v>600</v>
@@ -2458,7 +2443,7 @@
         <v>12000</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9">
         <v>7</v>
@@ -2469,10 +2454,10 @@
         <v>41295</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
       </c>
       <c r="D10">
         <v>415</v>
@@ -2481,21 +2466,21 @@
         <v>11050</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10">
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
       </c>
       <c r="D11">
         <v>360</v>
@@ -2504,7 +2489,7 @@
         <v>5000</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11">
         <v>4</v>
@@ -2512,24 +2497,27 @@
     </row>
     <row r="12" spans="1:8">
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
       </c>
       <c r="D12">
         <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
       </c>
       <c r="D13">
         <v>129</v>
@@ -2538,35 +2526,41 @@
         <v>3280</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15">
         <v>100</v>
@@ -2575,7 +2569,10 @@
         <v>2280</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2583,10 +2580,10 @@
         <v>41448</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16">
         <v>116</v>
@@ -2595,15 +2592,18 @@
         <v>3350</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17">
         <v>215</v>
@@ -2612,7 +2612,7 @@
         <v>4480</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>458</v>
       </c>
       <c r="G17">
         <v>3</v>
@@ -2620,10 +2620,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18">
         <v>108</v>
@@ -2632,15 +2632,18 @@
         <v>1700</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19">
         <v>86</v>
@@ -2649,15 +2652,18 @@
         <v>1600</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D20">
         <v>106</v>
@@ -2666,15 +2672,18 @@
         <v>2000</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="B21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <v>63</v>
@@ -2683,15 +2692,18 @@
         <v>1030</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="B22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D22">
         <v>100</v>
@@ -2700,26 +2712,32 @@
         <v>3000</v>
       </c>
       <c r="F22" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D24">
         <v>95</v>
@@ -2728,15 +2746,18 @@
         <v>2450</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="B25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25">
         <v>70</v>
@@ -2745,15 +2766,18 @@
         <v>2600</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="B26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26">
         <v>123</v>
@@ -2762,7 +2786,10 @@
         <v>3500</v>
       </c>
       <c r="F26" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2770,10 +2797,10 @@
         <v>41455</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D27">
         <v>106</v>
@@ -2782,7 +2809,10 @@
         <v>2600</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2790,10 +2820,10 @@
         <v>41448</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D28">
         <v>116</v>
@@ -2802,15 +2832,18 @@
         <v>3150</v>
       </c>
       <c r="F28" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="B29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D29">
         <v>108</v>
@@ -2819,15 +2852,18 @@
         <v>2740</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D30">
         <v>110</v>
@@ -2836,15 +2872,18 @@
         <v>3100</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="B31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D31">
         <v>100</v>
@@ -2853,15 +2892,18 @@
         <v>2600</v>
       </c>
       <c r="F31" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="B32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D32">
         <v>63</v>
@@ -2870,15 +2912,18 @@
         <v>2200</v>
       </c>
       <c r="F32" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D33">
         <v>102</v>
@@ -2887,15 +2932,18 @@
         <v>2550</v>
       </c>
       <c r="F33" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D34">
         <v>80</v>
@@ -2904,15 +2952,18 @@
         <v>1600</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35">
         <v>80</v>
@@ -2921,15 +2972,18 @@
         <v>2000</v>
       </c>
       <c r="F35" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D36">
         <v>109</v>
@@ -2938,7 +2992,10 @@
         <v>3730</v>
       </c>
       <c r="F36" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2946,10 +3003,10 @@
         <v>41403</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D37">
         <v>120</v>
@@ -2958,15 +3015,18 @@
         <v>2250</v>
       </c>
       <c r="F37" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="B38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D38">
         <v>84</v>
@@ -2975,7 +3035,10 @@
         <v>2200</v>
       </c>
       <c r="F38" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2983,10 +3046,10 @@
         <v>41385</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D39">
         <v>120</v>
@@ -2995,15 +3058,18 @@
         <v>2880</v>
       </c>
       <c r="F39" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D40">
         <v>83</v>
@@ -3012,15 +3078,18 @@
         <v>2290</v>
       </c>
       <c r="F40" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="B41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D41">
         <v>80</v>
@@ -3029,15 +3098,18 @@
         <v>2400</v>
       </c>
       <c r="F41" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="B42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D42">
         <v>83</v>
@@ -3046,15 +3118,18 @@
         <v>2000</v>
       </c>
       <c r="F42" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="B43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D43">
         <v>81</v>
@@ -3063,15 +3138,18 @@
         <v>2205</v>
       </c>
       <c r="F43" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D44">
         <v>220</v>
@@ -3080,7 +3158,7 @@
         <v>4900</v>
       </c>
       <c r="F44" t="s">
-        <v>42</v>
+        <v>458</v>
       </c>
       <c r="G44">
         <v>3</v>
@@ -3091,10 +3169,10 @@
         <v>41391</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D45">
         <v>100</v>
@@ -3103,15 +3181,18 @@
         <v>2300</v>
       </c>
       <c r="F45" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="B46" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D46">
         <v>63</v>
@@ -3120,15 +3201,18 @@
         <v>1600</v>
       </c>
       <c r="F46" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D47">
         <v>90</v>
@@ -3137,15 +3221,18 @@
         <v>2400</v>
       </c>
       <c r="F47" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="B48" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D48">
         <v>88</v>
@@ -3154,15 +3241,18 @@
         <v>2343</v>
       </c>
       <c r="F48" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="B49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D49">
         <v>80</v>
@@ -3171,15 +3261,18 @@
         <v>1900</v>
       </c>
       <c r="F49" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="B50" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D50">
         <v>76</v>
@@ -3188,15 +3281,18 @@
         <v>1900</v>
       </c>
       <c r="F50" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="B51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D51">
         <v>75</v>
@@ -3205,29 +3301,35 @@
         <v>2000</v>
       </c>
       <c r="F51" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="B52" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" t="s">
         <v>119</v>
       </c>
-      <c r="C52" t="s">
-        <v>120</v>
-      </c>
-      <c r="D52" t="s">
-        <v>121</v>
-      </c>
       <c r="F52" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="B53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D53">
         <v>107</v>
@@ -3236,15 +3338,18 @@
         <v>2150</v>
       </c>
       <c r="F53" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="B54" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D54">
         <v>101</v>
@@ -3253,15 +3358,18 @@
         <v>2650</v>
       </c>
       <c r="F54" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="B55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D55">
         <v>120</v>
@@ -3270,15 +3378,18 @@
         <v>3000</v>
       </c>
       <c r="F55" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="B56" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C56" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D56">
         <v>98</v>
@@ -3287,15 +3398,18 @@
         <v>3300</v>
       </c>
       <c r="F56" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="B57" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D57">
         <v>75</v>
@@ -3304,15 +3418,18 @@
         <v>1500</v>
       </c>
       <c r="F57" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="B58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C58" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D58">
         <v>103</v>
@@ -3321,15 +3438,18 @@
         <v>2700</v>
       </c>
       <c r="F58" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="B59" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D59">
         <v>56</v>
@@ -3338,15 +3458,18 @@
         <v>1436</v>
       </c>
       <c r="F59" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="B60" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C60" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D60">
         <v>117</v>
@@ -3355,15 +3478,18 @@
         <v>3100</v>
       </c>
       <c r="F60" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="B61" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D61">
         <v>102</v>
@@ -3372,15 +3498,18 @@
         <v>3600</v>
       </c>
       <c r="F61" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="B62" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C62" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D62">
         <v>86</v>
@@ -3389,7 +3518,10 @@
         <v>3600</v>
       </c>
       <c r="F62" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3397,10 +3529,10 @@
         <v>41430</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D63">
         <v>300</v>
@@ -3409,7 +3541,7 @@
         <v>10000</v>
       </c>
       <c r="F63" t="s">
-        <v>42</v>
+        <v>458</v>
       </c>
       <c r="G63">
         <v>4</v>
@@ -3417,10 +3549,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="B64" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D64">
         <v>102</v>
@@ -3429,15 +3561,18 @@
         <v>1820</v>
       </c>
       <c r="F64" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="B65" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C65" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D65">
         <v>85</v>
@@ -3446,7 +3581,10 @@
         <v>2000</v>
       </c>
       <c r="F65" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3454,10 +3592,10 @@
         <v>41392</v>
       </c>
       <c r="B66" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D66">
         <v>90</v>
@@ -3466,15 +3604,18 @@
         <v>2090</v>
       </c>
       <c r="F66" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="B67" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C67" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D67">
         <v>105</v>
@@ -3483,15 +3624,18 @@
         <v>2300</v>
       </c>
       <c r="F67" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="B68" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C68" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D68">
         <v>99</v>
@@ -3500,15 +3644,18 @@
         <v>2100</v>
       </c>
       <c r="F68" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="B69" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D69">
         <v>71</v>
@@ -3517,15 +3664,18 @@
         <v>2055</v>
       </c>
       <c r="F69" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="B70" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C70" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D70">
         <v>75</v>
@@ -3534,15 +3684,18 @@
         <v>1500</v>
       </c>
       <c r="F70" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="B71" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C71" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D71">
         <v>84</v>
@@ -3551,15 +3704,18 @@
         <v>2560</v>
       </c>
       <c r="F71" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="B72" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D72">
         <v>106</v>
@@ -3568,15 +3724,18 @@
         <v>2600</v>
       </c>
       <c r="F72" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="B73" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C73" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D73">
         <v>74</v>
@@ -3585,7 +3744,10 @@
         <v>2200</v>
       </c>
       <c r="F73" t="s">
-        <v>42</v>
+        <v>458</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3593,10 +3755,10 @@
         <v>41468</v>
       </c>
       <c r="B74" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C74" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D74">
         <v>598</v>
@@ -3605,7 +3767,7 @@
         <v>16685</v>
       </c>
       <c r="F74" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G74">
         <v>8</v>
@@ -3616,10 +3778,10 @@
         <v>41500</v>
       </c>
       <c r="B75" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C75" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D75">
         <v>552</v>
@@ -3628,7 +3790,7 @@
         <v>14800</v>
       </c>
       <c r="F75" t="s">
-        <v>42</v>
+        <v>458</v>
       </c>
       <c r="G75">
         <v>5</v>
@@ -3636,16 +3798,16 @@
     </row>
     <row r="76" spans="1:8">
       <c r="B76" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C76" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D76">
         <v>11000</v>
       </c>
       <c r="F76" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G76">
         <v>135</v>
@@ -3653,16 +3815,19 @@
     </row>
     <row r="77" spans="1:8">
       <c r="B77" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C77" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D77">
         <v>89</v>
       </c>
       <c r="F77" t="s">
-        <v>174</v>
+        <v>172</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3670,30 +3835,33 @@
         <v>41462</v>
       </c>
       <c r="B78" t="s">
+        <v>173</v>
+      </c>
+      <c r="C78" t="s">
+        <v>174</v>
+      </c>
+      <c r="D78" t="s">
         <v>175</v>
-      </c>
-      <c r="C78" t="s">
-        <v>176</v>
-      </c>
-      <c r="D78" t="s">
-        <v>177</v>
       </c>
       <c r="E78">
         <v>6600</v>
       </c>
       <c r="F78" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="B79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C79" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D79">
         <v>75</v>
@@ -3702,15 +3870,18 @@
         <v>2000</v>
       </c>
       <c r="F79" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="B80" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C80" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D80">
         <v>270</v>
@@ -3719,7 +3890,7 @@
         <v>9500</v>
       </c>
       <c r="F80" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G80">
         <v>4</v>
@@ -3727,10 +3898,10 @@
     </row>
     <row r="81" spans="1:7">
       <c r="B81" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C81" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D81">
         <v>175</v>
@@ -3739,7 +3910,7 @@
         <v>4100</v>
       </c>
       <c r="F81" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G81">
         <v>3</v>
@@ -3750,10 +3921,10 @@
         <v>41403</v>
       </c>
       <c r="B82" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C82" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D82">
         <v>223</v>
@@ -3762,7 +3933,7 @@
         <v>8000</v>
       </c>
       <c r="F82" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G82">
         <v>3</v>
@@ -3773,10 +3944,10 @@
         <v>41446</v>
       </c>
       <c r="B83" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C83" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D83">
         <v>130</v>
@@ -3785,7 +3956,7 @@
         <v>4000</v>
       </c>
       <c r="F83" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G83">
         <v>3</v>
@@ -3796,10 +3967,10 @@
         <v>41493</v>
       </c>
       <c r="B84" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C84" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D84">
         <v>200</v>
@@ -3808,7 +3979,7 @@
         <v>9150</v>
       </c>
       <c r="F84" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G84">
         <v>4</v>
@@ -3816,10 +3987,10 @@
     </row>
     <row r="85" spans="1:7">
       <c r="B85" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C85" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D85">
         <v>84</v>
@@ -3828,29 +3999,35 @@
         <v>2500</v>
       </c>
       <c r="F85" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="B86" t="s">
+        <v>192</v>
+      </c>
+      <c r="C86" t="s">
+        <v>193</v>
+      </c>
+      <c r="D86" t="s">
         <v>194</v>
       </c>
-      <c r="C86" t="s">
-        <v>195</v>
-      </c>
-      <c r="D86" t="s">
-        <v>196</v>
-      </c>
       <c r="F86" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="B87" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C87" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D87">
         <v>100</v>
@@ -3859,7 +4036,10 @@
         <v>2300</v>
       </c>
       <c r="F87" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -3867,41 +4047,47 @@
         <v>41419</v>
       </c>
       <c r="B88" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C88" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D88">
         <v>80</v>
       </c>
       <c r="F88" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="B89" t="s">
+        <v>199</v>
+      </c>
+      <c r="C89" t="s">
+        <v>200</v>
+      </c>
+      <c r="D89" t="s">
         <v>201</v>
-      </c>
-      <c r="C89" t="s">
-        <v>202</v>
-      </c>
-      <c r="D89" t="s">
-        <v>203</v>
       </c>
       <c r="E89">
         <v>1200</v>
       </c>
       <c r="F89" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="B90" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C90" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D90">
         <v>80</v>
@@ -3910,7 +4096,10 @@
         <v>2200</v>
       </c>
       <c r="F90" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -3918,27 +4107,30 @@
         <v>41462</v>
       </c>
       <c r="B91" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C91" t="s">
+        <v>174</v>
+      </c>
+      <c r="D91" t="s">
+        <v>175</v>
+      </c>
+      <c r="E91" t="s">
+        <v>205</v>
+      </c>
+      <c r="F91" t="s">
         <v>176</v>
       </c>
-      <c r="D91" t="s">
-        <v>177</v>
-      </c>
-      <c r="E91" t="s">
-        <v>207</v>
-      </c>
-      <c r="F91" t="s">
-        <v>178</v>
+      <c r="G91">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="B92" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C92" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D92">
         <v>85</v>
@@ -3947,46 +4139,55 @@
         <v>3800</v>
       </c>
       <c r="F92" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="B93" t="s">
+        <v>208</v>
+      </c>
+      <c r="C93" t="s">
+        <v>209</v>
+      </c>
+      <c r="D93" t="s">
         <v>210</v>
       </c>
-      <c r="C93" t="s">
-        <v>211</v>
-      </c>
-      <c r="D93" t="s">
-        <v>212</v>
-      </c>
       <c r="F93" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="B94" t="s">
+        <v>211</v>
+      </c>
+      <c r="C94" t="s">
+        <v>212</v>
+      </c>
+      <c r="D94" t="s">
+        <v>201</v>
+      </c>
+      <c r="E94" t="s">
         <v>213</v>
       </c>
-      <c r="C94" t="s">
-        <v>214</v>
-      </c>
-      <c r="D94" t="s">
-        <v>203</v>
-      </c>
-      <c r="E94" t="s">
-        <v>215</v>
-      </c>
       <c r="F94" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="B95" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C95" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D95">
         <v>105</v>
@@ -3995,15 +4196,18 @@
         <v>1740</v>
       </c>
       <c r="F95" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="B96" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C96" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D96">
         <v>160</v>
@@ -4012,7 +4216,7 @@
         <v>4000</v>
       </c>
       <c r="F96" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G96">
         <v>3</v>
@@ -4020,10 +4224,10 @@
     </row>
     <row r="97" spans="1:8">
       <c r="B97" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C97" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D97">
         <v>83</v>
@@ -4032,7 +4236,10 @@
         <v>2700</v>
       </c>
       <c r="F97" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4040,16 +4247,19 @@
         <v>41440</v>
       </c>
       <c r="B98" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C98" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D98">
         <v>85</v>
       </c>
       <c r="F98" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4057,10 +4267,10 @@
         <v>41371</v>
       </c>
       <c r="B99" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C99" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D99">
         <v>84</v>
@@ -4069,24 +4279,30 @@
         <v>2685</v>
       </c>
       <c r="F99" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="B100" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C100" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D100" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E100">
         <v>2600</v>
       </c>
       <c r="F100" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -4094,10 +4310,10 @@
         <v>41545</v>
       </c>
       <c r="B101" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C101" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D101">
         <v>320</v>
@@ -4106,7 +4322,7 @@
         <v>9500</v>
       </c>
       <c r="F101" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G101">
         <v>7</v>
@@ -4114,10 +4330,10 @@
     </row>
     <row r="102" spans="1:8">
       <c r="B102" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C102" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D102">
         <v>86</v>
@@ -4126,7 +4342,10 @@
         <v>3300</v>
       </c>
       <c r="F102" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4134,10 +4353,10 @@
         <v>41539</v>
       </c>
       <c r="B103" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C103" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D103">
         <v>112</v>
@@ -4146,13 +4365,13 @@
         <v>5150</v>
       </c>
       <c r="F103" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G103">
         <v>2</v>
       </c>
       <c r="H103" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4160,10 +4379,10 @@
         <v>41539</v>
       </c>
       <c r="B104" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C104" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D104">
         <v>112</v>
@@ -4172,15 +4391,18 @@
         <v>5150</v>
       </c>
       <c r="F104" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G104">
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="B105" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C105" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D105">
         <v>83</v>
@@ -4189,27 +4411,27 @@
         <v>2700</v>
       </c>
       <c r="F105" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H105" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="B106" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C106" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D106" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E106" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F106" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G106">
         <v>8</v>
@@ -4217,24 +4439,27 @@
     </row>
     <row r="107" spans="1:8">
       <c r="B107" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C107" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D107">
         <v>117</v>
       </c>
       <c r="F107" t="s">
-        <v>243</v>
+        <v>460</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="B108" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C108" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D108">
         <v>92</v>
@@ -4243,7 +4468,10 @@
         <v>3000</v>
       </c>
       <c r="F108" t="s">
-        <v>243</v>
+        <v>460</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4251,10 +4479,10 @@
         <v>41461</v>
       </c>
       <c r="B109" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C109" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D109">
         <v>110</v>
@@ -4263,7 +4491,10 @@
         <v>3350</v>
       </c>
       <c r="F109" t="s">
-        <v>248</v>
+        <v>457</v>
+      </c>
+      <c r="G109">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4271,10 +4502,10 @@
         <v>41399</v>
       </c>
       <c r="B110" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C110" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D110">
         <v>105</v>
@@ -4283,15 +4514,18 @@
         <v>3561</v>
       </c>
       <c r="F110" t="s">
-        <v>248</v>
+        <v>457</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:8">
       <c r="B111" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C111" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D111">
         <v>82</v>
@@ -4300,15 +4534,18 @@
         <v>4200</v>
       </c>
       <c r="F111" t="s">
-        <v>248</v>
+        <v>457</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:8">
       <c r="B112" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C112" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D112">
         <v>64</v>
@@ -4317,7 +4554,10 @@
         <v>2760</v>
       </c>
       <c r="F112" t="s">
-        <v>248</v>
+        <v>457</v>
+      </c>
+      <c r="G112">
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4325,10 +4565,10 @@
         <v>41461</v>
       </c>
       <c r="B113" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C113" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D113">
         <v>111</v>
@@ -4337,10 +4577,13 @@
         <v>3000</v>
       </c>
       <c r="F113" t="s">
-        <v>248</v>
+        <v>457</v>
+      </c>
+      <c r="G113">
+        <v>1</v>
       </c>
       <c r="H113" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4348,10 +4591,10 @@
         <v>41475</v>
       </c>
       <c r="B114" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C114" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D114">
         <v>650</v>
@@ -4360,7 +4603,7 @@
         <v>22000</v>
       </c>
       <c r="F114" t="s">
-        <v>248</v>
+        <v>457</v>
       </c>
       <c r="G114">
         <v>8</v>
@@ -4371,19 +4614,22 @@
         <v>41399</v>
       </c>
       <c r="B115" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C115" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D115" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E115">
         <v>2400</v>
       </c>
       <c r="F115" t="s">
-        <v>263</v>
+        <v>259</v>
+      </c>
+      <c r="G115">
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4391,10 +4637,10 @@
         <v>41406</v>
       </c>
       <c r="B116" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C116" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D116">
         <v>75</v>
@@ -4403,15 +4649,18 @@
         <v>2400</v>
       </c>
       <c r="F116" t="s">
-        <v>263</v>
+        <v>259</v>
+      </c>
+      <c r="G116">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:8">
       <c r="B117" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C117" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D117">
         <v>83</v>
@@ -4420,21 +4669,21 @@
         <v>1900</v>
       </c>
       <c r="F117" t="s">
-        <v>263</v>
+        <v>259</v>
+      </c>
+      <c r="G117">
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:8">
       <c r="B118" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C118" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D118">
         <v>700</v>
-      </c>
-      <c r="F118" t="s">
-        <v>269</v>
       </c>
       <c r="G118">
         <v>7</v>
@@ -4445,22 +4694,22 @@
         <v>41349</v>
       </c>
       <c r="B119" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C119" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D119">
         <v>250</v>
       </c>
       <c r="F119" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="G119">
         <v>5</v>
       </c>
       <c r="H119" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4468,10 +4717,10 @@
         <v>41516</v>
       </c>
       <c r="B120" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C120" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D120">
         <v>1400</v>
@@ -4480,7 +4729,7 @@
         <v>14000</v>
       </c>
       <c r="F120" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="G120">
         <v>9</v>
@@ -4491,16 +4740,16 @@
         <v>41413</v>
       </c>
       <c r="B121" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C121" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D121">
         <v>440</v>
       </c>
       <c r="F121" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="G121">
         <v>6</v>
@@ -4511,38 +4760,44 @@
         <v>41343</v>
       </c>
       <c r="B122" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C122" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D122">
         <v>90</v>
       </c>
       <c r="F122" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G122">
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:8">
       <c r="B123" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C123" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D123">
         <v>65</v>
       </c>
       <c r="F123" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G123">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:8">
       <c r="B124" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C124" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D124">
         <v>100</v>
@@ -4551,7 +4806,10 @@
         <v>2200</v>
       </c>
       <c r="F124" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G124">
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -4559,47 +4817,56 @@
         <v>41343</v>
       </c>
       <c r="B125" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C125" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D125" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F125" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G125">
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:8">
       <c r="B126" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C126" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D126">
         <v>80</v>
       </c>
       <c r="F126" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G126">
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:8">
-      <c r="A127" t="s">
-        <v>292</v>
+      <c r="A127" s="1">
+        <v>41356</v>
       </c>
       <c r="B127" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C127" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D127" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F127" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -4607,44 +4874,53 @@
         <v>41238</v>
       </c>
       <c r="B128" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C128" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D128">
         <v>75</v>
       </c>
       <c r="F128" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G128">
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:8">
       <c r="B129" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C129" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D129">
         <v>55</v>
       </c>
       <c r="F129" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G129">
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:8">
       <c r="B130" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C130" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D130" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F130" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G130">
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -4652,10 +4928,10 @@
         <v>41337</v>
       </c>
       <c r="B131" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C131" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D131">
         <v>70</v>
@@ -4664,24 +4940,30 @@
         <v>1350</v>
       </c>
       <c r="F131" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
       </c>
       <c r="H131" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="132" spans="1:8">
       <c r="B132" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C132" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D132" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F132" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -4689,10 +4971,10 @@
         <v>41306</v>
       </c>
       <c r="B133" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C133" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D133">
         <v>259</v>
@@ -4701,35 +4983,38 @@
         <v>5250</v>
       </c>
       <c r="F133" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G133">
         <v>5</v>
       </c>
       <c r="H133" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="134" spans="1:8">
       <c r="B134" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C134" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D134">
         <v>94</v>
       </c>
       <c r="F134" t="s">
-        <v>314</v>
+        <v>308</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:8">
       <c r="B135" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C135" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D135">
         <v>540</v>
@@ -4738,7 +5023,7 @@
         <v>4648</v>
       </c>
       <c r="F135" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="G135">
         <v>3</v>
@@ -4746,10 +5031,10 @@
     </row>
     <row r="136" spans="1:8">
       <c r="B136" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C136" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D136">
         <v>64</v>
@@ -4758,7 +5043,10 @@
         <v>2400</v>
       </c>
       <c r="F136" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G136">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -4766,10 +5054,10 @@
         <v>41424</v>
       </c>
       <c r="B137" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C137" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D137">
         <v>211</v>
@@ -4778,7 +5066,7 @@
         <v>8200</v>
       </c>
       <c r="F137" t="s">
-        <v>320</v>
+        <v>456</v>
       </c>
       <c r="G137">
         <v>4</v>
@@ -4786,10 +5074,10 @@
     </row>
     <row r="138" spans="1:8">
       <c r="B138" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C138" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D138">
         <v>100</v>
@@ -4798,15 +5086,18 @@
         <v>3000</v>
       </c>
       <c r="F138" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G138">
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:8">
       <c r="B139" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C139" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D139">
         <v>90</v>
@@ -4815,15 +5106,18 @@
         <v>3060</v>
       </c>
       <c r="F139" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G139">
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:8">
       <c r="B140" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C140" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D140">
         <v>104</v>
@@ -4832,15 +5126,18 @@
         <v>3800</v>
       </c>
       <c r="F140" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G140">
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:8">
       <c r="B141" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C141" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D141">
         <v>78</v>
@@ -4849,15 +5146,18 @@
         <v>2750</v>
       </c>
       <c r="F141" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:8">
       <c r="B142" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C142" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D142">
         <v>70</v>
@@ -4866,15 +5166,18 @@
         <v>2050</v>
       </c>
       <c r="F142" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G142">
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:8">
       <c r="B143" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C143" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D143">
         <v>79</v>
@@ -4883,7 +5186,10 @@
         <v>3820</v>
       </c>
       <c r="F143" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G143">
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -4891,10 +5197,10 @@
         <v>41454</v>
       </c>
       <c r="B144" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C144" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D144">
         <v>95</v>
@@ -4903,15 +5209,18 @@
         <v>4400</v>
       </c>
       <c r="F144" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G144">
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:8">
       <c r="B145" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C145" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D145">
         <v>72</v>
@@ -4920,15 +5229,18 @@
         <v>1600</v>
       </c>
       <c r="F145" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:8">
       <c r="B146" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C146" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D146">
         <v>75</v>
@@ -4937,15 +5249,18 @@
         <v>2500</v>
       </c>
       <c r="F146" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G146">
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:8">
       <c r="B147" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C147" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="D147">
         <v>80</v>
@@ -4954,15 +5269,18 @@
         <v>1570</v>
       </c>
       <c r="F147" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G147">
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:8">
       <c r="B148" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="C148" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D148">
         <v>119</v>
@@ -4971,15 +5289,18 @@
         <v>3800</v>
       </c>
       <c r="F148" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:8">
       <c r="B149" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C149" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D149">
         <v>210</v>
@@ -4988,15 +5309,18 @@
         <v>7000</v>
       </c>
       <c r="F149" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G149">
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:8">
       <c r="B150" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C150" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D150">
         <v>72</v>
@@ -5005,15 +5329,18 @@
         <v>2700</v>
       </c>
       <c r="F150" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G150">
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:8">
       <c r="B151" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C151" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="D151">
         <v>71</v>
@@ -5022,15 +5349,18 @@
         <v>2170</v>
       </c>
       <c r="F151" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G151">
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:8">
       <c r="B152" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="C152" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="D152">
         <v>66</v>
@@ -5039,15 +5369,18 @@
         <v>2300</v>
       </c>
       <c r="F152" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G152">
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:8">
       <c r="B153" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="C153" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D153">
         <v>64</v>
@@ -5056,15 +5389,18 @@
         <v>2000</v>
       </c>
       <c r="F153" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G153">
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:8">
       <c r="B154" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C154" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="D154">
         <v>74</v>
@@ -5073,15 +5409,18 @@
         <v>3500</v>
       </c>
       <c r="F154" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G154">
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:8">
       <c r="B155" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="C155" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D155">
         <v>70</v>
@@ -5090,15 +5429,18 @@
         <v>1450</v>
       </c>
       <c r="F155" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:8">
       <c r="B156" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C156" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D156">
         <v>80</v>
@@ -5107,15 +5449,18 @@
         <v>3678</v>
       </c>
       <c r="F156" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:8">
       <c r="B157" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C157" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="D157">
         <v>203</v>
@@ -5124,13 +5469,13 @@
         <v>10046</v>
       </c>
       <c r="F157" t="s">
-        <v>320</v>
+        <v>456</v>
       </c>
       <c r="G157">
         <v>3</v>
       </c>
       <c r="H157" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5138,10 +5483,10 @@
         <v>41304</v>
       </c>
       <c r="B158" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C158" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="D158">
         <v>335</v>
@@ -5150,21 +5495,21 @@
         <v>4650</v>
       </c>
       <c r="F158" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G158">
         <v>4</v>
       </c>
       <c r="H158" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="159" spans="1:8">
       <c r="B159" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C159" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D159">
         <v>145</v>
@@ -5173,18 +5518,21 @@
         <v>4400</v>
       </c>
       <c r="F159" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G159">
+        <v>1</v>
       </c>
       <c r="H159" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="160" spans="1:8">
       <c r="B160" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="C160" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D160">
         <v>208</v>
@@ -5193,10 +5541,13 @@
         <v>7000</v>
       </c>
       <c r="F160" t="s">
-        <v>320</v>
+        <v>456</v>
+      </c>
+      <c r="G160">
+        <v>1</v>
       </c>
       <c r="H160" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5204,10 +5555,10 @@
         <v>41455</v>
       </c>
       <c r="B161" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="C161" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="D161">
         <v>285</v>
@@ -5216,7 +5567,7 @@
         <v>9270</v>
       </c>
       <c r="F161" t="s">
-        <v>371</v>
+        <v>456</v>
       </c>
       <c r="G161">
         <v>5</v>
@@ -5227,10 +5578,10 @@
         <v>41439</v>
       </c>
       <c r="B162" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C162" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D162">
         <v>103</v>
@@ -5239,7 +5590,7 @@
         <v>1900</v>
       </c>
       <c r="F162" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="G162">
         <v>3</v>
@@ -5247,10 +5598,10 @@
     </row>
     <row r="163" spans="1:8">
       <c r="B163" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="C163" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="D163">
         <v>400</v>
@@ -5259,13 +5610,13 @@
         <v>12000</v>
       </c>
       <c r="F163" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="G163">
         <v>6</v>
       </c>
       <c r="H163" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -5273,10 +5624,10 @@
         <v>41399</v>
       </c>
       <c r="B164" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C164" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="D164">
         <v>426</v>
@@ -5285,33 +5636,33 @@
         <v>9125</v>
       </c>
       <c r="F164" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G164">
         <v>5</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
     </row>
     <row r="165" spans="1:8">
       <c r="B165" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C165" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D165">
         <v>700</v>
       </c>
       <c r="F165" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G165">
         <v>7</v>
       </c>
       <c r="H165" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -5319,10 +5670,10 @@
         <v>41398</v>
       </c>
       <c r="B166" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C166" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="D166">
         <v>1150</v>
@@ -5331,13 +5682,13 @@
         <v>21000</v>
       </c>
       <c r="F166" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G166">
         <v>9</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -5345,30 +5696,30 @@
         <v>41341</v>
       </c>
       <c r="B167" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C167" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D167">
         <v>550</v>
       </c>
       <c r="F167" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="G167">
         <v>10</v>
       </c>
       <c r="H167" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
     </row>
     <row r="168" spans="1:8">
       <c r="B168" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="C168" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="D168">
         <v>85</v>
@@ -5377,18 +5728,21 @@
         <v>3000</v>
       </c>
       <c r="F168" t="s">
-        <v>389</v>
+        <v>381</v>
+      </c>
+      <c r="G168">
+        <v>1</v>
       </c>
       <c r="H168" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="169" spans="1:8">
       <c r="B169" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C169" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="D169">
         <v>104</v>
@@ -5397,10 +5751,13 @@
         <v>3300</v>
       </c>
       <c r="F169" t="s">
-        <v>392</v>
+        <v>384</v>
+      </c>
+      <c r="G169">
+        <v>1</v>
       </c>
       <c r="H169" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -5408,10 +5765,10 @@
         <v>41329</v>
       </c>
       <c r="B170" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C170" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="D170">
         <v>410</v>
@@ -5420,30 +5777,33 @@
         <v>12000</v>
       </c>
       <c r="F170" t="s">
-        <v>395</v>
+        <v>455</v>
       </c>
       <c r="G170">
         <v>6</v>
       </c>
       <c r="H170" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="171" spans="1:8">
       <c r="B171" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="C171" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="D171">
         <v>80</v>
       </c>
       <c r="F171" t="s">
-        <v>395</v>
+        <v>455</v>
+      </c>
+      <c r="G171">
+        <v>1</v>
       </c>
       <c r="H171" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -5451,10 +5811,10 @@
         <v>41370</v>
       </c>
       <c r="B172" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="C172" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="D172">
         <v>85</v>
@@ -5463,10 +5823,13 @@
         <v>2350</v>
       </c>
       <c r="F172" t="s">
-        <v>395</v>
+        <v>455</v>
+      </c>
+      <c r="G172">
+        <v>1</v>
       </c>
       <c r="H172" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -5474,10 +5837,10 @@
         <v>41461</v>
       </c>
       <c r="B173" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="C173" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="D173">
         <v>820</v>
@@ -5486,21 +5849,21 @@
         <v>20000</v>
       </c>
       <c r="F173" t="s">
-        <v>395</v>
+        <v>455</v>
       </c>
       <c r="G173">
         <v>8</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="174" spans="1:8">
       <c r="B174" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="C174" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="D174">
         <v>102</v>
@@ -5509,38 +5872,41 @@
         <v>2690</v>
       </c>
       <c r="F174" t="s">
-        <v>405</v>
+        <v>396</v>
+      </c>
+      <c r="G174">
+        <v>1</v>
       </c>
       <c r="H174" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
     <row r="175" spans="1:8">
       <c r="B175" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="C175" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="D175">
         <v>220</v>
       </c>
       <c r="F175" t="s">
-        <v>408</v>
+        <v>454</v>
       </c>
       <c r="G175">
         <v>3</v>
       </c>
       <c r="H175" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
     </row>
     <row r="176" spans="1:8">
       <c r="B176" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="C176" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="D176">
         <v>101</v>
@@ -5549,18 +5915,21 @@
         <v>3600</v>
       </c>
       <c r="F176" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G176">
+        <v>1</v>
       </c>
       <c r="H176" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
     </row>
     <row r="177" spans="1:8">
       <c r="B177" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="C177" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="D177">
         <v>87</v>
@@ -5569,7 +5938,10 @@
         <v>3300</v>
       </c>
       <c r="F177" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G177">
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5577,10 +5949,10 @@
         <v>41350</v>
       </c>
       <c r="B178" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="C178" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="D178">
         <v>698</v>
@@ -5589,21 +5961,21 @@
         <v>15900</v>
       </c>
       <c r="F178" t="s">
-        <v>416</v>
+        <v>459</v>
       </c>
       <c r="G178">
         <v>8</v>
       </c>
       <c r="H178" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
     </row>
     <row r="179" spans="1:8">
       <c r="B179" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="C179" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="D179">
         <v>91</v>
@@ -5612,18 +5984,21 @@
         <v>4800</v>
       </c>
       <c r="F179" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G179">
+        <v>1</v>
       </c>
       <c r="H179" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
     </row>
     <row r="180" spans="1:8">
       <c r="B180" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="C180" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="D180">
         <v>72</v>
@@ -5632,18 +6007,21 @@
         <v>3200</v>
       </c>
       <c r="F180" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G180">
+        <v>1</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
     </row>
     <row r="181" spans="1:8">
       <c r="B181" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="C181" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="D181">
         <v>88</v>
@@ -5652,18 +6030,21 @@
         <v>3900</v>
       </c>
       <c r="F181" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G181">
+        <v>1</v>
       </c>
       <c r="H181" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
     </row>
     <row r="182" spans="1:8">
       <c r="B182" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="C182" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D182">
         <v>83</v>
@@ -5672,18 +6053,21 @@
         <v>2600</v>
       </c>
       <c r="F182" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G182">
+        <v>1</v>
       </c>
       <c r="H182" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
     </row>
     <row r="183" spans="1:8">
       <c r="B183" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="C183" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D183">
         <v>60</v>
@@ -5692,18 +6076,21 @@
         <v>1450</v>
       </c>
       <c r="F183" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G183">
+        <v>1</v>
       </c>
       <c r="H183" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
     </row>
     <row r="184" spans="1:8">
       <c r="B184" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="C184" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D184">
         <v>94</v>
@@ -5712,10 +6099,13 @@
         <v>3500</v>
       </c>
       <c r="F184" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G184">
+        <v>1</v>
       </c>
       <c r="H184" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5723,10 +6113,10 @@
         <v>41517</v>
       </c>
       <c r="B185" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="C185" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D185">
         <v>138</v>
@@ -5735,10 +6125,13 @@
         <v>4010</v>
       </c>
       <c r="F185" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G185">
+        <v>1</v>
       </c>
       <c r="H185" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5746,10 +6139,10 @@
         <v>41504</v>
       </c>
       <c r="B186" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="C186" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D186">
         <v>400</v>
@@ -5758,13 +6151,13 @@
         <v>12900</v>
       </c>
       <c r="F186" t="s">
-        <v>433</v>
+        <v>453</v>
       </c>
       <c r="G186">
         <v>6</v>
       </c>
       <c r="H186" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5772,10 +6165,10 @@
         <v>41509</v>
       </c>
       <c r="B187" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="C187" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="D187">
         <v>145</v>
@@ -5784,10 +6177,13 @@
         <v>5800</v>
       </c>
       <c r="F187" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G187">
+        <v>1</v>
       </c>
       <c r="H187" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5795,10 +6191,10 @@
         <v>41517</v>
       </c>
       <c r="B188" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="C188" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D188">
         <v>138</v>
@@ -5807,10 +6203,13 @@
         <v>4010</v>
       </c>
       <c r="F188" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G188">
+        <v>1</v>
       </c>
       <c r="H188" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5818,10 +6217,10 @@
         <v>41476</v>
       </c>
       <c r="B189" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="C189" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="D189">
         <v>105</v>
@@ -5830,15 +6229,13 @@
         <v>4400</v>
       </c>
       <c r="F189" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="G189">
+        <v>1</v>
       </c>
       <c r="H189" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1">
-      <c r="A193" t="s">
-        <v>464</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>